<commit_message>
Cadastro da idéia do Radé
</commit_message>
<xml_diff>
--- a/Empreendimentos/Backlog de Empreendimentos.xlsx
+++ b/Empreendimentos/Backlog de Empreendimentos.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>#</t>
   </si>
@@ -61,6 +61,12 @@
   </si>
   <si>
     <t>Em Implementação</t>
+  </si>
+  <si>
+    <t>Plataforma para venda e compra de ingressos</t>
+  </si>
+  <si>
+    <t>Vinícius Radé</t>
   </si>
 </sst>
 </file>
@@ -413,7 +419,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -486,6 +492,26 @@
         <v>10</v>
       </c>
     </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="1">
+        <v>42544</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>